<commit_message>
Added random primms data
</commit_message>
<xml_diff>
--- a/resultData/sampleData.xlsx
+++ b/resultData/sampleData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19310"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caevol\Desktop\multiagent\resultData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD9639C-2004-4821-A03B-A79CB97D58B8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35AC87FE-DBF3-4EB4-922A-5987673FB439}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{F63F76EB-9BA6-4EA9-8AC4-955003381E79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179016"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,30 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
-  <si>
-    <t>Pop</t>
-  </si>
-  <si>
-    <t>Geo</t>
-  </si>
-  <si>
-    <t>Voronoi</t>
-  </si>
-  <si>
-    <t>Primms</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
   <si>
     <t>Small Input</t>
   </si>
   <si>
     <t>Large Input</t>
-  </si>
-  <si>
-    <t>MEAN</t>
-  </si>
-  <si>
-    <t>STDEV</t>
   </si>
   <si>
     <t>Commited Primms Normal Size</t>
@@ -60,17 +42,38 @@
     <t>Small City Pop</t>
   </si>
   <si>
+    <t>Big City Pop</t>
+  </si>
+  <si>
+    <t>Random Primms</t>
+  </si>
+  <si>
+    <t>Voronoi</t>
+  </si>
+  <si>
+    <t>Primms</t>
+  </si>
+  <si>
     <t>Vornoi</t>
   </si>
   <si>
-    <t>Big City Pop</t>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Geo</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>STDEV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,147 +433,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C54FDF2-308E-444B-BBA3-EBA5EEB3AC2B}">
-  <dimension ref="A6:AJ31"/>
+  <dimension ref="A6:AP31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="AI8" sqref="AI8:AJ31"/>
+    <sheetView tabSelected="1" topLeftCell="AE5" workbookViewId="0" xr3:uid="{FB83F964-9415-575F-9EFE-F1EE9242F103}">
+      <selection activeCell="AL30" sqref="AL30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42">
       <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
+      <c r="AF6" t="s">
         <v>5</v>
       </c>
-      <c r="N6" t="s">
+      <c r="AL6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:42">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="T6" t="s">
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" t="s">
+        <v>7</v>
+      </c>
+      <c r="W8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8" t="s">
         <v>9</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AC8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:42">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="AF6" t="s">
-        <v>12</v>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" t="s">
+        <v>10</v>
+      </c>
+      <c r="U9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W9" t="s">
+        <v>10</v>
+      </c>
+      <c r="X9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>3</v>
-      </c>
-      <c r="T8" t="s">
-        <v>2</v>
-      </c>
-      <c r="W8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>1</v>
-      </c>
-      <c r="T9" t="s">
-        <v>0</v>
-      </c>
-      <c r="U9" t="s">
-        <v>1</v>
-      </c>
-      <c r="W9" t="s">
-        <v>0</v>
-      </c>
-      <c r="X9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42">
       <c r="B10">
         <v>1</v>
       </c>
@@ -643,8 +667,20 @@
       <c r="AJ10">
         <v>0.77190000000000003</v>
       </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <v>0.96779999999999999</v>
+      </c>
+      <c r="AO10">
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <v>0.87929999999999997</v>
+      </c>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42">
       <c r="B11">
         <v>1</v>
       </c>
@@ -717,8 +753,20 @@
       <c r="AJ11">
         <v>0.78210000000000002</v>
       </c>
+      <c r="AL11">
+        <v>1</v>
+      </c>
+      <c r="AM11">
+        <v>0.8649</v>
+      </c>
+      <c r="AO11">
+        <v>1</v>
+      </c>
+      <c r="AP11">
+        <v>0.78800000000000003</v>
+      </c>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42">
       <c r="B12">
         <v>0.75</v>
       </c>
@@ -791,8 +839,20 @@
       <c r="AJ12">
         <v>0.64480000000000004</v>
       </c>
+      <c r="AL12">
+        <v>0.625</v>
+      </c>
+      <c r="AM12">
+        <v>0.89990000000000003</v>
+      </c>
+      <c r="AO12">
+        <v>0.75</v>
+      </c>
+      <c r="AP12">
+        <v>0.81320000000000003</v>
+      </c>
     </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42">
       <c r="B13">
         <v>0.75</v>
       </c>
@@ -865,8 +925,20 @@
       <c r="AJ13">
         <v>0.72840000000000005</v>
       </c>
+      <c r="AL13">
+        <v>0.875</v>
+      </c>
+      <c r="AM13">
+        <v>0.9254</v>
+      </c>
+      <c r="AO13">
+        <v>0.875</v>
+      </c>
+      <c r="AP13">
+        <v>0.84470000000000001</v>
+      </c>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42">
       <c r="B14">
         <v>0.75</v>
       </c>
@@ -939,8 +1011,20 @@
       <c r="AJ14">
         <v>0.73980000000000001</v>
       </c>
+      <c r="AL14">
+        <v>0.75</v>
+      </c>
+      <c r="AM14">
+        <v>0.88590000000000002</v>
+      </c>
+      <c r="AO14">
+        <v>0.875</v>
+      </c>
+      <c r="AP14">
+        <v>0.81889999999999996</v>
+      </c>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42">
       <c r="B15">
         <v>0.75</v>
       </c>
@@ -1013,8 +1097,20 @@
       <c r="AJ15">
         <v>0.80210000000000004</v>
       </c>
+      <c r="AL15">
+        <v>0.75</v>
+      </c>
+      <c r="AM15">
+        <v>0.9325</v>
+      </c>
+      <c r="AO15">
+        <v>0.75</v>
+      </c>
+      <c r="AP15">
+        <v>0.84660000000000002</v>
+      </c>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42">
       <c r="B16">
         <v>1</v>
       </c>
@@ -1087,8 +1183,20 @@
       <c r="AJ16">
         <v>0.77170000000000005</v>
       </c>
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AM16">
+        <v>0.90469999999999995</v>
+      </c>
+      <c r="AO16">
+        <v>1</v>
+      </c>
+      <c r="AP16">
+        <v>0.84289999999999998</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42">
       <c r="B17">
         <v>0.25</v>
       </c>
@@ -1161,8 +1269,20 @@
       <c r="AJ17">
         <v>0.85370000000000001</v>
       </c>
+      <c r="AL17">
+        <v>0.875</v>
+      </c>
+      <c r="AM17">
+        <v>0.96360000000000001</v>
+      </c>
+      <c r="AO17">
+        <v>0.75</v>
+      </c>
+      <c r="AP17">
+        <v>0.89829999999999999</v>
+      </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42">
       <c r="B18">
         <v>0.75</v>
       </c>
@@ -1235,8 +1355,20 @@
       <c r="AJ18">
         <v>0.75570000000000004</v>
       </c>
+      <c r="AL18">
+        <v>0.875</v>
+      </c>
+      <c r="AM18">
+        <v>0.87590000000000001</v>
+      </c>
+      <c r="AO18">
+        <v>0.875</v>
+      </c>
+      <c r="AP18">
+        <v>0.78979999999999995</v>
+      </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42">
       <c r="B19">
         <v>0.75</v>
       </c>
@@ -1309,8 +1441,20 @@
       <c r="AJ19">
         <v>0.77110000000000001</v>
       </c>
+      <c r="AL19">
+        <v>0.75</v>
+      </c>
+      <c r="AM19">
+        <v>0.86580000000000001</v>
+      </c>
+      <c r="AO19">
+        <v>0.875</v>
+      </c>
+      <c r="AP19">
+        <v>0.8206</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42">
       <c r="B20">
         <v>0.75</v>
       </c>
@@ -1383,8 +1527,20 @@
       <c r="AJ20">
         <v>0.76100000000000001</v>
       </c>
+      <c r="AL20">
+        <v>1</v>
+      </c>
+      <c r="AM20">
+        <v>0.96640000000000004</v>
+      </c>
+      <c r="AO20">
+        <v>1</v>
+      </c>
+      <c r="AP20">
+        <v>0.89710000000000001</v>
+      </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42">
       <c r="B21">
         <v>0.75</v>
       </c>
@@ -1457,8 +1613,20 @@
       <c r="AJ21">
         <v>0.63</v>
       </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AM21">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
+      <c r="AP21">
+        <v>0.90290000000000004</v>
+      </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42">
       <c r="B22">
         <v>0.25</v>
       </c>
@@ -1531,8 +1699,20 @@
       <c r="AJ22">
         <v>0.76</v>
       </c>
+      <c r="AL22">
+        <v>0.875</v>
+      </c>
+      <c r="AM22">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="AO22">
+        <v>1</v>
+      </c>
+      <c r="AP22">
+        <v>0.77329999999999999</v>
+      </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42">
       <c r="B23">
         <v>0.5</v>
       </c>
@@ -1605,8 +1785,20 @@
       <c r="AJ23">
         <v>0.80769999999999997</v>
       </c>
+      <c r="AL23">
+        <v>1</v>
+      </c>
+      <c r="AM23">
+        <v>0.8881</v>
+      </c>
+      <c r="AO23">
+        <v>1</v>
+      </c>
+      <c r="AP23">
+        <v>0.80559999999999998</v>
+      </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1679,8 +1871,20 @@
       <c r="AJ24">
         <v>0.74519999999999997</v>
       </c>
+      <c r="AL24">
+        <v>1</v>
+      </c>
+      <c r="AM24">
+        <v>0.92769999999999997</v>
+      </c>
+      <c r="AO24">
+        <v>1</v>
+      </c>
+      <c r="AP24">
+        <v>0.85919999999999996</v>
+      </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42">
       <c r="B25">
         <v>0.5</v>
       </c>
@@ -1753,8 +1957,20 @@
       <c r="AJ25">
         <v>0.79339999999999999</v>
       </c>
+      <c r="AL25">
+        <v>0.875</v>
+      </c>
+      <c r="AM25">
+        <v>0.96</v>
+      </c>
+      <c r="AO25">
+        <v>0.875</v>
+      </c>
+      <c r="AP25">
+        <v>0.877</v>
+      </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42">
       <c r="B26">
         <v>0.75</v>
       </c>
@@ -1827,8 +2043,20 @@
       <c r="AJ26">
         <v>0.7006</v>
       </c>
+      <c r="AL26">
+        <v>0.75</v>
+      </c>
+      <c r="AM26">
+        <v>0.96440000000000003</v>
+      </c>
+      <c r="AO26">
+        <v>0.75</v>
+      </c>
+      <c r="AP26">
+        <v>0.88109999999999999</v>
+      </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42">
       <c r="B27">
         <v>1</v>
       </c>
@@ -1901,8 +2129,20 @@
       <c r="AJ27">
         <v>0.67169999999999996</v>
       </c>
+      <c r="AL27">
+        <v>0.75</v>
+      </c>
+      <c r="AM27">
+        <v>0.86950000000000005</v>
+      </c>
+      <c r="AO27">
+        <v>0.75</v>
+      </c>
+      <c r="AP27">
+        <v>0.78259999999999996</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42">
       <c r="B28">
         <v>0.5</v>
       </c>
@@ -1975,8 +2215,20 @@
       <c r="AJ28">
         <v>0.82469999999999999</v>
       </c>
+      <c r="AL28">
+        <v>1</v>
+      </c>
+      <c r="AM28">
+        <v>0.96230000000000004</v>
+      </c>
+      <c r="AO28">
+        <v>1</v>
+      </c>
+      <c r="AP28">
+        <v>0.87519999999999998</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42">
       <c r="B29">
         <v>1</v>
       </c>
@@ -2049,10 +2301,22 @@
       <c r="AJ29">
         <v>0.76949999999999996</v>
       </c>
+      <c r="AL29">
+        <v>0.875</v>
+      </c>
+      <c r="AM29">
+        <v>0.88</v>
+      </c>
+      <c r="AO29">
+        <v>0.75</v>
+      </c>
+      <c r="AP29">
+        <v>0.7923</v>
+      </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42">
       <c r="A30" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1">
         <f>AVERAGE(B10:B29)</f>
@@ -2158,10 +2422,26 @@
         <f>AVERAGE(AJ10:AJ29)</f>
         <v>0.75425500000000012</v>
       </c>
+      <c r="AL30" s="1">
+        <f>AVERAGE(AL10:AL29)</f>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="AM30" s="1">
+        <f>AVERAGE(AM10:AM29)</f>
+        <v>0.91428999999999994</v>
+      </c>
+      <c r="AO30" s="1">
+        <f>AVERAGE(AO10:AO29)</f>
+        <v>0.89375000000000004</v>
+      </c>
+      <c r="AP30" s="1">
+        <f>AVERAGE(AP10:AP29)</f>
+        <v>0.83943000000000012</v>
+      </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42">
       <c r="A31" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B31" s="1">
         <f>STDEV(B10:B29)</f>
@@ -2266,6 +2546,22 @@
       <c r="AJ31" s="1">
         <f>STDEV(AJ10:AJ29)</f>
         <v>5.6935203012769386E-2</v>
+      </c>
+      <c r="AL31" s="1">
+        <f>STDEV(AL10:AL29)</f>
+        <v>0.11806415517354174</v>
+      </c>
+      <c r="AM31" s="1">
+        <f>STDEV(AM10:AM29)</f>
+        <v>4.5667135482290712E-2</v>
+      </c>
+      <c r="AO31" s="1">
+        <f>STDEV(AO10:AO29)</f>
+        <v>0.10938674748942741</v>
+      </c>
+      <c r="AP31" s="1">
+        <f>STDEV(AP10:AP29)</f>
+        <v>4.2833706599506804E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>